<commit_message>
updated icons and query reporter
</commit_message>
<xml_diff>
--- a/data-raw/info organismi marini_rev.xlsx
+++ b/data-raw/info organismi marini_rev.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Desktop\ADViSEBioassay\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B31822-C98E-4D43-8075-B12047C84D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C311453F-8101-4910-8CBF-AECE75E79944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="624">
   <si>
     <t>EXP</t>
   </si>
@@ -264,9 +264,6 @@
     <t>Mollusca</t>
   </si>
   <si>
-    <t>0- meters</t>
-  </si>
-  <si>
     <t>CBC280A</t>
   </si>
   <si>
@@ -1316,9 +1313,6 @@
     <t>Myriaporidae</t>
   </si>
   <si>
-    <t>Valerio Mazzella Ischia</t>
-  </si>
-  <si>
     <t>CBC184A</t>
   </si>
   <si>
@@ -1808,10 +1802,6 @@
   </si>
   <si>
     <t>ADV41</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fusaro lake Casina Vanvitelliana
-</t>
   </si>
   <si>
     <t xml:space="preserve">0-200 meters
@@ -1965,6 +1955,10 @@
   </si>
   <si>
     <t>Mergellina Baia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fusaro lake Casina Vanvitelliana
+</t>
   </si>
 </sst>
 </file>
@@ -2000,18 +1994,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2041,7 +2029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2057,22 +2045,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2355,10 +2328,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
@@ -2412,19 +2385,19 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="M1" s="12" t="s">
+        <v>614</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>19</v>
@@ -2462,7 +2435,7 @@
         <v>17</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="N2">
         <v>3.9</v>
@@ -2520,7 +2493,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -2544,7 +2517,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="M4" s="4">
         <v>44014</v>
@@ -2629,7 +2602,7 @@
         <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>47</v>
@@ -2693,7 +2666,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C8" t="s">
         <v>59</v>
@@ -2717,10 +2690,10 @@
         <v>16</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M8" s="4">
         <v>43991</v>
@@ -2761,16 +2734,16 @@
         <v>16</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>73</v>
+        <v>548</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="M9" s="5">
         <v>44397</v>
       </c>
       <c r="O9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2778,16 +2751,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
         <v>75</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>76</v>
-      </c>
-      <c r="E10" t="s">
-        <v>77</v>
       </c>
       <c r="F10" t="s">
         <v>70</v>
@@ -2802,16 +2775,16 @@
         <v>16</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="N10">
         <v>4</v>
       </c>
       <c r="O10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2819,34 +2792,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
         <v>80</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>81</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>82</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>83</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>84</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>85</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I11" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="K11" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>55</v>
@@ -2858,7 +2831,7 @@
         <v>80</v>
       </c>
       <c r="O11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2866,34 +2839,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
         <v>91</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>92</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>93</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>94</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>95</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="M12" s="5">
         <v>44306</v>
@@ -2902,7 +2875,7 @@
         <v>34</v>
       </c>
       <c r="O12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2910,19 +2883,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" t="s">
         <v>99</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>100</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>101</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>102</v>
-      </c>
-      <c r="F13" t="s">
-        <v>103</v>
       </c>
       <c r="G13" t="s">
         <v>71</v>
@@ -2934,10 +2907,10 @@
         <v>16</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M13" s="5">
         <v>44352</v>
@@ -2946,95 +2919,95 @@
         <v>40</v>
       </c>
       <c r="O13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="E14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M14" s="4">
+        <v>44245</v>
+      </c>
+      <c r="N14">
+        <v>90</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>13</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>606</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="14" t="s">
+      <c r="B15" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" s="14" t="s">
+      <c r="G15" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H15" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>621</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="M14" s="15">
-        <v>44245</v>
-      </c>
-      <c r="N14" s="14">
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M15" s="4">
+        <v>44386</v>
+      </c>
+      <c r="N15">
         <v>90</v>
       </c>
-      <c r="O14" s="13" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
-        <v>13</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>606</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="M15" s="15">
-        <v>44386</v>
-      </c>
-      <c r="N15" s="14">
-        <v>90</v>
-      </c>
-      <c r="O15" s="13" t="s">
-        <v>622</v>
+      <c r="O15" s="3" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3042,19 +3015,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
         <v>106</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>107</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>108</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>109</v>
-      </c>
-      <c r="F16" t="s">
-        <v>110</v>
       </c>
       <c r="G16" t="s">
         <v>71</v>
@@ -3066,19 +3039,19 @@
         <v>16</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="L16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M16" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="N16">
         <v>70</v>
       </c>
       <c r="O16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -3086,40 +3059,40 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" t="s">
         <v>114</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>115</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>116</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>117</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>118</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>119</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="I17" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="M17" s="5">
         <v>44310</v>
       </c>
       <c r="P17" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3127,34 +3100,34 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
         <v>123</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>124</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>125</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>126</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="G18" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" t="s">
-        <v>96</v>
-      </c>
-      <c r="I18" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="M18" s="5">
         <v>43809</v>
@@ -3163,7 +3136,7 @@
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3171,34 +3144,34 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" t="s">
         <v>130</v>
       </c>
-      <c r="C19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" t="s">
+        <v>95</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E19" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" t="s">
-        <v>127</v>
-      </c>
-      <c r="G19" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" t="s">
-        <v>96</v>
-      </c>
-      <c r="I19" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="L19" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M19" s="5">
         <v>44439</v>
@@ -3207,7 +3180,7 @@
         <v>24</v>
       </c>
       <c r="O19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -3215,34 +3188,34 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" t="s">
         <v>134</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>135</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="E20" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20" t="s">
-        <v>96</v>
-      </c>
-      <c r="I20" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="M20" s="5">
         <v>43809</v>
@@ -3251,7 +3224,7 @@
         <v>4</v>
       </c>
       <c r="O20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -3259,34 +3232,34 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" t="s">
         <v>139</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>140</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>141</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>142</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>143</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H21" t="s">
-        <v>120</v>
-      </c>
-      <c r="I21" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="M21" s="5">
         <v>43809</v>
@@ -3295,7 +3268,7 @@
         <v>885</v>
       </c>
       <c r="O21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3303,43 +3276,43 @@
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" t="s">
+        <v>147</v>
+      </c>
+      <c r="E22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" t="s">
+        <v>143</v>
+      </c>
+      <c r="H22" t="s">
+        <v>119</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="M22" s="4" t="s">
         <v>572</v>
-      </c>
-      <c r="C22" t="s">
-        <v>140</v>
-      </c>
-      <c r="D22" t="s">
-        <v>148</v>
-      </c>
-      <c r="E22" t="s">
-        <v>142</v>
-      </c>
-      <c r="F22" t="s">
-        <v>143</v>
-      </c>
-      <c r="G22" t="s">
-        <v>144</v>
-      </c>
-      <c r="H22" t="s">
-        <v>120</v>
-      </c>
-      <c r="I22" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>573</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>574</v>
       </c>
       <c r="N22" s="3">
         <v>48</v>
       </c>
       <c r="O22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -3347,19 +3320,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" t="s">
         <v>150</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>151</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>152</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>153</v>
-      </c>
-      <c r="F23" t="s">
-        <v>154</v>
       </c>
       <c r="G23" t="s">
         <v>71</v>
@@ -3371,7 +3344,7 @@
         <v>16</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M23" s="5">
         <v>44246</v>
@@ -3382,31 +3355,31 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" t="s">
         <v>156</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>157</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>158</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>159</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="G24" t="s">
-        <v>95</v>
-      </c>
-      <c r="H24" t="s">
-        <v>96</v>
-      </c>
-      <c r="I24" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="M24" s="5">
         <v>43647</v>
@@ -3415,7 +3388,7 @@
         <v>52</v>
       </c>
       <c r="O24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3423,34 +3396,34 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" t="s">
         <v>163</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>164</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>165</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>166</v>
       </c>
-      <c r="F25" t="s">
-        <v>167</v>
-      </c>
       <c r="G25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" t="s">
         <v>85</v>
       </c>
-      <c r="H25" t="s">
-        <v>86</v>
-      </c>
       <c r="I25" t="s">
         <v>16</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M25" s="5">
         <v>44043</v>
@@ -3459,7 +3432,7 @@
         <v>70</v>
       </c>
       <c r="O25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3467,46 +3440,46 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D26" t="s">
+        <v>168</v>
+      </c>
+      <c r="E26" t="s">
+        <v>165</v>
+      </c>
+      <c r="F26" t="s">
+        <v>166</v>
+      </c>
+      <c r="G26" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="O26" t="s">
         <v>169</v>
-      </c>
-      <c r="E26" t="s">
-        <v>166</v>
-      </c>
-      <c r="F26" t="s">
-        <v>167</v>
-      </c>
-      <c r="G26" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26" t="s">
-        <v>86</v>
-      </c>
-      <c r="I26" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="O26" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -3514,19 +3487,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>174</v>
+      </c>
+      <c r="C27" t="s">
         <v>175</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>176</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>177</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>178</v>
-      </c>
-      <c r="F27" t="s">
-        <v>179</v>
       </c>
       <c r="G27" t="s">
         <v>63</v>
@@ -3538,10 +3511,10 @@
         <v>16</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M27" s="5">
         <v>44251</v>
@@ -3550,7 +3523,7 @@
         <v>57</v>
       </c>
       <c r="O27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -3558,19 +3531,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C28" t="s">
         <v>182</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>183</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>184</v>
       </c>
-      <c r="E28" t="s">
-        <v>185</v>
-      </c>
       <c r="F28" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G28" t="s">
         <v>71</v>
@@ -3582,7 +3555,7 @@
         <v>16</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="M28" s="5">
         <v>43996</v>
@@ -3591,7 +3564,7 @@
         <v>38</v>
       </c>
       <c r="O28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -3599,19 +3572,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29" t="s">
         <v>188</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>189</v>
       </c>
-      <c r="D29" t="s">
-        <v>190</v>
-      </c>
       <c r="E29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" t="s">
         <v>102</v>
-      </c>
-      <c r="F29" t="s">
-        <v>103</v>
       </c>
       <c r="G29" t="s">
         <v>71</v>
@@ -3623,10 +3596,10 @@
         <v>16</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M29" s="5">
         <v>44371</v>
@@ -3635,7 +3608,7 @@
         <v>180</v>
       </c>
       <c r="O29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3643,13 +3616,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C30" t="s">
         <v>192</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>193</v>
-      </c>
-      <c r="D30" t="s">
-        <v>194</v>
       </c>
       <c r="E30" t="s">
         <v>24</v>
@@ -3667,19 +3640,19 @@
         <v>16</v>
       </c>
       <c r="J30" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="L30" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="M30" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="M30" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="N30" s="3">
         <v>57</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -3687,19 +3660,19 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
+        <v>198</v>
+      </c>
+      <c r="C31" t="s">
         <v>199</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>200</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>201</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>202</v>
-      </c>
-      <c r="F31" t="s">
-        <v>203</v>
       </c>
       <c r="G31" t="s">
         <v>71</v>
@@ -3711,19 +3684,19 @@
         <v>16</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="L31" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="M31" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="M31" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="N31">
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -3731,43 +3704,43 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="C32" t="s">
+        <v>206</v>
+      </c>
+      <c r="D32" t="s">
+        <v>207</v>
+      </c>
+      <c r="E32" t="s">
+        <v>208</v>
+      </c>
+      <c r="F32" t="s">
+        <v>209</v>
+      </c>
+      <c r="G32" t="s">
+        <v>546</v>
+      </c>
+      <c r="H32" t="s">
+        <v>210</v>
+      </c>
+      <c r="I32" t="s">
+        <v>211</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="M32" s="4" t="s">
         <v>577</v>
-      </c>
-      <c r="C32" t="s">
-        <v>207</v>
-      </c>
-      <c r="D32" t="s">
-        <v>208</v>
-      </c>
-      <c r="E32" t="s">
-        <v>209</v>
-      </c>
-      <c r="F32" t="s">
-        <v>210</v>
-      </c>
-      <c r="G32" t="s">
-        <v>548</v>
-      </c>
-      <c r="H32" t="s">
-        <v>211</v>
-      </c>
-      <c r="I32" t="s">
-        <v>212</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>578</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>579</v>
-      </c>
-      <c r="M32" s="4" t="s">
-        <v>580</v>
       </c>
       <c r="N32" s="3">
         <v>43</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -3775,16 +3748,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C33" t="s">
         <v>214</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>215</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>216</v>
-      </c>
-      <c r="E33" t="s">
-        <v>217</v>
       </c>
       <c r="F33" t="s">
         <v>25</v>
@@ -3799,10 +3772,10 @@
         <v>16</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M33" s="5">
         <v>44256</v>
@@ -3811,7 +3784,7 @@
         <v>36</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -3819,19 +3792,19 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" t="s">
         <v>220</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>221</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>222</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>223</v>
-      </c>
-      <c r="F34" t="s">
-        <v>224</v>
       </c>
       <c r="G34" t="s">
         <v>71</v>
@@ -3843,10 +3816,10 @@
         <v>16</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M34" s="5">
         <v>44256</v>
@@ -3857,19 +3830,19 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>224</v>
+      </c>
+      <c r="C35" t="s">
+        <v>220</v>
+      </c>
+      <c r="D35" t="s">
         <v>225</v>
       </c>
-      <c r="C35" t="s">
-        <v>221</v>
-      </c>
-      <c r="D35" t="s">
-        <v>226</v>
-      </c>
       <c r="E35" t="s">
+        <v>222</v>
+      </c>
+      <c r="F35" t="s">
         <v>223</v>
-      </c>
-      <c r="F35" t="s">
-        <v>224</v>
       </c>
       <c r="G35" t="s">
         <v>71</v>
@@ -3881,10 +3854,10 @@
         <v>16</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M35" s="5">
         <v>43996</v>
@@ -3898,31 +3871,31 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
+        <v>227</v>
+      </c>
+      <c r="C36" t="s">
         <v>228</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>229</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>230</v>
       </c>
-      <c r="E36" t="s">
-        <v>231</v>
-      </c>
       <c r="G36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H36" t="s">
         <v>85</v>
       </c>
-      <c r="H36" t="s">
-        <v>86</v>
-      </c>
       <c r="I36" t="s">
         <v>16</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M36" s="5">
         <v>43996</v>
@@ -3931,7 +3904,7 @@
         <v>34</v>
       </c>
       <c r="O36" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -3939,34 +3912,34 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>232</v>
+      </c>
+      <c r="C37" t="s">
         <v>233</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>234</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>235</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>236</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>237</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>238</v>
       </c>
-      <c r="H37" t="s">
-        <v>239</v>
-      </c>
       <c r="I37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M37" s="5">
         <v>44302</v>
@@ -3977,19 +3950,19 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>239</v>
+      </c>
+      <c r="C38" t="s">
         <v>240</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>241</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>242</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>243</v>
-      </c>
-      <c r="F38" t="s">
-        <v>244</v>
       </c>
       <c r="G38" t="s">
         <v>14</v>
@@ -4001,13 +3974,13 @@
         <v>16</v>
       </c>
       <c r="J38" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="K38" t="s">
         <v>245</v>
       </c>
-      <c r="K38" t="s">
-        <v>246</v>
-      </c>
       <c r="L38" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M38" s="8">
         <v>44048</v>
@@ -4021,19 +3994,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C39" t="s">
+        <v>246</v>
+      </c>
+      <c r="D39" t="s">
         <v>247</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>248</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>249</v>
-      </c>
-      <c r="F39" t="s">
-        <v>250</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
@@ -4045,19 +4018,19 @@
         <v>16</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="K39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M39" s="4">
         <v>42856</v>
       </c>
       <c r="O39" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4065,37 +4038,37 @@
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="C40" t="s">
+        <v>251</v>
+      </c>
+      <c r="D40" t="s">
+        <v>252</v>
+      </c>
+      <c r="E40" t="s">
+        <v>253</v>
+      </c>
+      <c r="F40" t="s">
+        <v>254</v>
+      </c>
+      <c r="G40" t="s">
+        <v>94</v>
+      </c>
+      <c r="H40" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="L40" s="3" t="s">
         <v>584</v>
-      </c>
-      <c r="C40" t="s">
-        <v>252</v>
-      </c>
-      <c r="D40" t="s">
-        <v>253</v>
-      </c>
-      <c r="E40" t="s">
-        <v>254</v>
-      </c>
-      <c r="F40" t="s">
-        <v>255</v>
-      </c>
-      <c r="G40" t="s">
-        <v>95</v>
-      </c>
-      <c r="H40" t="s">
-        <v>96</v>
-      </c>
-      <c r="I40" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>585</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>587</v>
       </c>
       <c r="M40" s="4">
         <v>43996</v>
@@ -4104,7 +4077,7 @@
         <v>19</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -4112,19 +4085,19 @@
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C41" t="s">
+        <v>258</v>
+      </c>
+      <c r="D41" t="s">
+        <v>257</v>
+      </c>
+      <c r="E41" t="s">
         <v>259</v>
       </c>
-      <c r="D41" t="s">
-        <v>258</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>260</v>
-      </c>
-      <c r="F41" t="s">
-        <v>261</v>
       </c>
       <c r="G41" t="s">
         <v>26</v>
@@ -4136,7 +4109,7 @@
         <v>16</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M41" s="5">
         <v>43250</v>
@@ -4145,7 +4118,7 @@
         <v>72</v>
       </c>
       <c r="O41" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -4153,34 +4126,34 @@
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C42" t="s">
         <v>264</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>265</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>266</v>
       </c>
-      <c r="E42" t="s">
-        <v>267</v>
-      </c>
       <c r="F42" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" t="s">
         <v>94</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>95</v>
       </c>
-      <c r="H42" t="s">
-        <v>96</v>
-      </c>
       <c r="I42" t="s">
         <v>16</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M42" s="5">
         <v>43991</v>
@@ -4189,7 +4162,7 @@
         <v>17</v>
       </c>
       <c r="O42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -4197,34 +4170,34 @@
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C43" t="s">
+        <v>268</v>
+      </c>
+      <c r="D43" t="s">
         <v>269</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>270</v>
       </c>
-      <c r="E43" t="s">
-        <v>271</v>
-      </c>
       <c r="F43" t="s">
+        <v>209</v>
+      </c>
+      <c r="G43" t="s">
+        <v>546</v>
+      </c>
+      <c r="H43" t="s">
         <v>210</v>
       </c>
-      <c r="G43" t="s">
-        <v>548</v>
-      </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>211</v>
       </c>
-      <c r="I43" t="s">
-        <v>212</v>
-      </c>
       <c r="J43" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="M43" s="4">
         <v>44250</v>
@@ -4233,7 +4206,7 @@
         <v>41</v>
       </c>
       <c r="O43" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -4241,34 +4214,34 @@
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C44" t="s">
+        <v>268</v>
+      </c>
+      <c r="D44" t="s">
         <v>273</v>
       </c>
-      <c r="C44" t="s">
-        <v>269</v>
-      </c>
-      <c r="D44" t="s">
-        <v>274</v>
-      </c>
       <c r="E44" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F44" t="s">
+        <v>209</v>
+      </c>
+      <c r="G44" t="s">
+        <v>546</v>
+      </c>
+      <c r="H44" t="s">
         <v>210</v>
       </c>
-      <c r="G44" t="s">
-        <v>548</v>
-      </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>211</v>
       </c>
-      <c r="I44" t="s">
-        <v>212</v>
-      </c>
       <c r="J44" s="3" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M44" s="5">
         <v>44371</v>
@@ -4279,34 +4252,34 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C45" t="s">
+        <v>274</v>
+      </c>
+      <c r="D45" t="s">
         <v>275</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>276</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>277</v>
       </c>
-      <c r="F45" t="s">
-        <v>278</v>
-      </c>
       <c r="G45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I45" t="s">
         <v>16</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="M45" s="4">
         <v>44305</v>
@@ -4315,7 +4288,7 @@
         <v>25</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -4323,16 +4296,16 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C46" t="s">
         <v>280</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>281</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>282</v>
-      </c>
-      <c r="E46" t="s">
-        <v>283</v>
       </c>
       <c r="F46" t="s">
         <v>70</v>
@@ -4347,16 +4320,16 @@
         <v>16</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M46" s="5">
         <v>44251</v>
       </c>
       <c r="O46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -4364,16 +4337,16 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C47" t="s">
         <v>285</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>286</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>287</v>
-      </c>
-      <c r="E47" t="s">
-        <v>288</v>
       </c>
       <c r="F47" t="s">
         <v>70</v>
@@ -4388,10 +4361,10 @@
         <v>16</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M47" s="5">
         <v>44251</v>
@@ -4400,7 +4373,7 @@
         <v>33</v>
       </c>
       <c r="O47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -4408,31 +4381,31 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C48" t="s">
+        <v>289</v>
+      </c>
+      <c r="D48" t="s">
         <v>290</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>291</v>
       </c>
-      <c r="E48" t="s">
-        <v>292</v>
-      </c>
       <c r="F48" t="s">
+        <v>93</v>
+      </c>
+      <c r="G48" t="s">
         <v>94</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>95</v>
       </c>
-      <c r="H48" t="s">
-        <v>96</v>
-      </c>
       <c r="I48" t="s">
         <v>16</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="5">
@@ -4442,7 +4415,7 @@
         <v>118</v>
       </c>
       <c r="O48" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -4450,31 +4423,31 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C49" t="s">
+        <v>289</v>
+      </c>
+      <c r="D49" t="s">
         <v>290</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>291</v>
       </c>
-      <c r="E49" t="s">
-        <v>292</v>
-      </c>
       <c r="F49" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" t="s">
         <v>94</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>95</v>
       </c>
-      <c r="H49" t="s">
-        <v>96</v>
-      </c>
       <c r="I49" t="s">
         <v>16</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="M49" s="4">
         <v>43811</v>
@@ -4483,7 +4456,7 @@
         <v>55</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -4491,34 +4464,34 @@
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C50" t="s">
         <v>293</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>294</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>295</v>
       </c>
-      <c r="E50" t="s">
-        <v>296</v>
-      </c>
       <c r="F50" t="s">
+        <v>93</v>
+      </c>
+      <c r="G50" t="s">
         <v>94</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>95</v>
       </c>
-      <c r="H50" t="s">
-        <v>96</v>
-      </c>
       <c r="I50" t="s">
         <v>16</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M50" s="5">
         <v>43996</v>
@@ -4527,7 +4500,7 @@
         <v>60</v>
       </c>
       <c r="O50" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -4535,16 +4508,16 @@
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C51" t="s">
         <v>298</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>299</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>300</v>
-      </c>
-      <c r="E51" t="s">
-        <v>301</v>
       </c>
       <c r="F51" t="s">
         <v>70</v>
@@ -4559,7 +4532,7 @@
         <v>16</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M51" s="5">
         <v>43647</v>
@@ -4568,48 +4541,48 @@
         <v>25</v>
       </c>
       <c r="O51" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
-        <v>50</v>
-      </c>
-      <c r="B52" s="10" t="s">
+      <c r="C52" t="s">
         <v>304</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="D52" t="s">
         <v>305</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="E52" t="s">
         <v>306</v>
       </c>
-      <c r="E52" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" t="s">
         <v>70</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G52" t="s">
         <v>71</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="H52" t="s">
         <v>72</v>
       </c>
-      <c r="I52" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>604</v>
-      </c>
-      <c r="L52" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="M52" s="11">
+      <c r="I52" t="s">
+        <v>16</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M52" s="4">
         <v>44439</v>
       </c>
-      <c r="O52" s="10" t="s">
-        <v>605</v>
+      <c r="O52" s="3" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -4617,34 +4590,34 @@
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C53" t="s">
         <v>308</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>309</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>310</v>
       </c>
-      <c r="E53" t="s">
-        <v>311</v>
-      </c>
       <c r="F53" t="s">
+        <v>209</v>
+      </c>
+      <c r="G53" t="s">
+        <v>546</v>
+      </c>
+      <c r="H53" t="s">
         <v>210</v>
       </c>
-      <c r="G53" t="s">
-        <v>548</v>
-      </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>211</v>
       </c>
-      <c r="I53" t="s">
-        <v>212</v>
-      </c>
       <c r="J53" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="L53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M53" s="5">
         <v>44048</v>
@@ -4653,7 +4626,7 @@
         <v>33</v>
       </c>
       <c r="O53" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -4661,19 +4634,19 @@
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C54" t="s">
         <v>313</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>314</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>315</v>
       </c>
-      <c r="E54" t="s">
-        <v>316</v>
-      </c>
       <c r="F54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G54" t="s">
         <v>71</v>
@@ -4685,19 +4658,19 @@
         <v>16</v>
       </c>
       <c r="J54" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="M54" s="4" t="s">
         <v>317</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="M54" s="4" t="s">
-        <v>318</v>
       </c>
       <c r="N54">
         <v>138</v>
       </c>
       <c r="O54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -4705,19 +4678,19 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C55" t="s">
         <v>321</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>322</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>323</v>
       </c>
-      <c r="E55" t="s">
-        <v>324</v>
-      </c>
       <c r="F55" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G55" t="s">
         <v>71</v>
@@ -4729,10 +4702,10 @@
         <v>16</v>
       </c>
       <c r="J55" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="L55" t="s">
         <v>325</v>
-      </c>
-      <c r="L55" t="s">
-        <v>326</v>
       </c>
       <c r="M55" s="5">
         <v>43768</v>
@@ -4741,7 +4714,7 @@
         <v>5</v>
       </c>
       <c r="O55" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -4749,16 +4722,16 @@
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C56" t="s">
         <v>328</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>329</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>330</v>
-      </c>
-      <c r="E56" t="s">
-        <v>331</v>
       </c>
       <c r="F56" t="s">
         <v>70</v>
@@ -4773,10 +4746,10 @@
         <v>16</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M56" s="5">
         <v>44256</v>
@@ -4785,7 +4758,7 @@
         <v>12</v>
       </c>
       <c r="O56" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -4793,34 +4766,34 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C57" t="s">
         <v>334</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>335</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>336</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>337</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>338</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>339</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
+        <v>16</v>
+      </c>
+      <c r="J57" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="I57" t="s">
-        <v>16</v>
-      </c>
-      <c r="J57" s="3" t="s">
+      <c r="L57" t="s">
         <v>341</v>
-      </c>
-      <c r="L57" t="s">
-        <v>342</v>
       </c>
       <c r="M57" s="5">
         <v>44348</v>
@@ -4829,7 +4802,7 @@
         <v>300</v>
       </c>
       <c r="O57" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -4837,22 +4810,22 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C58" t="s">
         <v>344</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>345</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>346</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>347</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>348</v>
-      </c>
-      <c r="G58" t="s">
-        <v>349</v>
       </c>
       <c r="H58" t="s">
         <v>72</v>
@@ -4861,10 +4834,10 @@
         <v>16</v>
       </c>
       <c r="J58" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="L58" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="L58" s="3" t="s">
-        <v>351</v>
       </c>
       <c r="M58" s="5">
         <v>44186</v>
@@ -4873,7 +4846,7 @@
         <v>116</v>
       </c>
       <c r="O58" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -4881,19 +4854,19 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C59" t="s">
         <v>353</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>354</v>
       </c>
-      <c r="D59" t="s">
-        <v>355</v>
-      </c>
       <c r="E59" t="s">
+        <v>346</v>
+      </c>
+      <c r="F59" t="s">
         <v>347</v>
-      </c>
-      <c r="F59" t="s">
-        <v>348</v>
       </c>
       <c r="G59" t="s">
         <v>71</v>
@@ -4905,10 +4878,10 @@
         <v>16</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M59" s="5">
         <v>44258</v>
@@ -4917,7 +4890,7 @@
         <v>28</v>
       </c>
       <c r="O59" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -4925,19 +4898,19 @@
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C60" t="s">
+        <v>353</v>
+      </c>
+      <c r="D60" t="s">
         <v>357</v>
       </c>
-      <c r="C60" t="s">
-        <v>354</v>
-      </c>
-      <c r="D60" t="s">
-        <v>358</v>
-      </c>
       <c r="E60" t="s">
+        <v>346</v>
+      </c>
+      <c r="F60" t="s">
         <v>347</v>
-      </c>
-      <c r="F60" t="s">
-        <v>348</v>
       </c>
       <c r="G60" t="s">
         <v>71</v>
@@ -4949,10 +4922,10 @@
         <v>16</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M60" s="5">
         <v>43810</v>
@@ -4961,7 +4934,7 @@
         <v>37</v>
       </c>
       <c r="O60" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -4969,19 +4942,19 @@
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C61" t="s">
+        <v>359</v>
+      </c>
+      <c r="D61" t="s">
         <v>360</v>
       </c>
-      <c r="D61" t="s">
-        <v>361</v>
-      </c>
       <c r="E61" t="s">
+        <v>152</v>
+      </c>
+      <c r="F61" t="s">
         <v>153</v>
-      </c>
-      <c r="F61" t="s">
-        <v>154</v>
       </c>
       <c r="G61" t="s">
         <v>71</v>
@@ -4993,10 +4966,10 @@
         <v>16</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M61" s="4">
         <v>43809</v>
@@ -5005,7 +4978,7 @@
         <v>40</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -5013,34 +4986,34 @@
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C62" t="s">
         <v>363</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>364</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>365</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>366</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>367</v>
       </c>
-      <c r="G62" t="s">
-        <v>368</v>
-      </c>
       <c r="H62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I62" t="s">
         <v>16</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M62" s="5">
         <v>43996</v>
@@ -5049,7 +5022,7 @@
         <v>200</v>
       </c>
       <c r="O62" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -5057,37 +5030,37 @@
         <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C63" t="s">
+        <v>363</v>
+      </c>
+      <c r="D63" t="s">
         <v>370</v>
       </c>
-      <c r="C63" t="s">
-        <v>364</v>
-      </c>
-      <c r="D63" t="s">
-        <v>371</v>
-      </c>
       <c r="E63" t="s">
+        <v>365</v>
+      </c>
+      <c r="F63" t="s">
         <v>366</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>367</v>
       </c>
-      <c r="G63" t="s">
-        <v>368</v>
-      </c>
       <c r="H63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I63" t="s">
         <v>16</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="K63" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M63" s="5">
         <v>44048</v>
@@ -5096,7 +5069,7 @@
         <v>124</v>
       </c>
       <c r="O63" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -5104,34 +5077,34 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C64" t="s">
+        <v>363</v>
+      </c>
+      <c r="D64" t="s">
         <v>373</v>
       </c>
-      <c r="C64" t="s">
-        <v>364</v>
-      </c>
-      <c r="D64" t="s">
-        <v>374</v>
-      </c>
       <c r="E64" t="s">
+        <v>365</v>
+      </c>
+      <c r="F64" t="s">
         <v>366</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>367</v>
       </c>
-      <c r="G64" t="s">
-        <v>368</v>
-      </c>
       <c r="H64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I64" t="s">
         <v>16</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M64" s="5">
         <v>43996</v>
@@ -5140,7 +5113,7 @@
         <v>115</v>
       </c>
       <c r="O64" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
@@ -5148,31 +5121,31 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C65" t="s">
         <v>376</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>377</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>378</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>379</v>
       </c>
-      <c r="F65" t="s">
-        <v>380</v>
-      </c>
       <c r="G65" t="s">
+        <v>237</v>
+      </c>
+      <c r="H65" t="s">
         <v>238</v>
       </c>
-      <c r="H65" t="s">
-        <v>239</v>
-      </c>
       <c r="I65" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="M65" s="5">
         <v>44097</v>
@@ -5181,7 +5154,7 @@
         <v>232</v>
       </c>
       <c r="O65" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
@@ -5189,16 +5162,16 @@
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C66" t="s">
         <v>382</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>383</v>
       </c>
-      <c r="D66" t="s">
-        <v>384</v>
-      </c>
       <c r="E66" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F66" t="s">
         <v>53</v>
@@ -5213,13 +5186,13 @@
         <v>16</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K66" t="s">
+        <v>386</v>
+      </c>
+      <c r="L66" s="3" t="s">
         <v>387</v>
-      </c>
-      <c r="L66" s="3" t="s">
-        <v>388</v>
       </c>
       <c r="M66" s="5">
         <v>43525</v>
@@ -5228,7 +5201,7 @@
         <v>166</v>
       </c>
       <c r="O66" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
@@ -5236,22 +5209,22 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C67" t="s">
         <v>390</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>391</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>392</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>393</v>
       </c>
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>394</v>
-      </c>
-      <c r="G67" t="s">
-        <v>395</v>
       </c>
       <c r="H67" t="s">
         <v>27</v>
@@ -5260,10 +5233,10 @@
         <v>16</v>
       </c>
       <c r="J67" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="L67" s="3" t="s">
         <v>396</v>
-      </c>
-      <c r="L67" s="3" t="s">
-        <v>397</v>
       </c>
       <c r="M67" s="5">
         <v>44409</v>
@@ -5272,7 +5245,7 @@
         <v>7</v>
       </c>
       <c r="O67" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
@@ -5280,37 +5253,37 @@
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C68" t="s">
+        <v>398</v>
+      </c>
+      <c r="D68" t="s">
         <v>399</v>
       </c>
-      <c r="D68" t="s">
-        <v>400</v>
-      </c>
       <c r="E68" t="s">
+        <v>276</v>
+      </c>
+      <c r="F68" t="s">
         <v>277</v>
       </c>
-      <c r="F68" t="s">
-        <v>278</v>
-      </c>
       <c r="G68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H68" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I68" t="s">
         <v>16</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="M68" s="4">
         <v>44500</v>
@@ -5319,7 +5292,7 @@
         <v>21</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
@@ -5327,34 +5300,34 @@
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C69" t="s">
         <v>402</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>403</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>404</v>
       </c>
-      <c r="E69" t="s">
-        <v>405</v>
-      </c>
       <c r="F69" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G69" t="s">
+        <v>94</v>
+      </c>
+      <c r="H69" t="s">
         <v>95</v>
       </c>
-      <c r="H69" t="s">
-        <v>96</v>
-      </c>
       <c r="I69" t="s">
         <v>16</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M69" s="5">
         <v>44251</v>
@@ -5363,7 +5336,7 @@
         <v>87</v>
       </c>
       <c r="O69" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
@@ -5371,19 +5344,19 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C70" t="s">
         <v>407</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>408</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>409</v>
       </c>
-      <c r="E70" t="s">
-        <v>410</v>
-      </c>
       <c r="F70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G70" t="s">
         <v>71</v>
@@ -5395,54 +5368,54 @@
         <v>16</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M70" s="5">
         <v>44382</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C71" t="s">
         <v>412</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="D71" t="s">
         <v>413</v>
       </c>
-      <c r="D71" s="14" t="s">
+      <c r="E71" t="s">
         <v>414</v>
       </c>
-      <c r="E71" s="14" t="s">
+      <c r="F71" t="s">
+        <v>178</v>
+      </c>
+      <c r="G71" t="s">
+        <v>63</v>
+      </c>
+      <c r="H71" t="s">
+        <v>64</v>
+      </c>
+      <c r="I71" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M71" s="5">
+        <v>44014</v>
+      </c>
+      <c r="N71">
+        <v>54</v>
+      </c>
+      <c r="O71" t="s">
         <v>415</v>
-      </c>
-      <c r="F71" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="G71" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="H71" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I71" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J71" s="13" t="s">
-        <v>416</v>
-      </c>
-      <c r="M71" s="16">
-        <v>44014</v>
-      </c>
-      <c r="N71" s="14">
-        <v>54</v>
-      </c>
-      <c r="O71" s="14" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
@@ -5450,34 +5423,34 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
+        <v>416</v>
+      </c>
+      <c r="C72" t="s">
+        <v>417</v>
+      </c>
+      <c r="D72" t="s">
         <v>418</v>
       </c>
-      <c r="C72" t="s">
-        <v>419</v>
-      </c>
-      <c r="D72" t="s">
-        <v>420</v>
-      </c>
       <c r="E72" t="s">
+        <v>165</v>
+      </c>
+      <c r="F72" t="s">
         <v>166</v>
       </c>
-      <c r="F72" t="s">
-        <v>167</v>
-      </c>
       <c r="G72" t="s">
+        <v>84</v>
+      </c>
+      <c r="H72" t="s">
         <v>85</v>
       </c>
-      <c r="H72" t="s">
-        <v>86</v>
-      </c>
       <c r="I72" t="s">
         <v>16</v>
       </c>
       <c r="J72" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="L72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M72" s="5">
         <v>44397</v>
@@ -5488,19 +5461,19 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C73" t="s">
+        <v>420</v>
+      </c>
+      <c r="D73" t="s">
         <v>421</v>
       </c>
-      <c r="C73" t="s">
+      <c r="E73" t="s">
         <v>422</v>
       </c>
-      <c r="D73" t="s">
-        <v>423</v>
-      </c>
-      <c r="E73" t="s">
-        <v>424</v>
-      </c>
       <c r="F73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G73" t="s">
         <v>71</v>
@@ -5512,10 +5485,10 @@
         <v>16</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="L73" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="M73" s="5">
         <v>44258</v>
@@ -5526,34 +5499,34 @@
         <v>72</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C74" t="s">
+        <v>426</v>
+      </c>
+      <c r="D74" t="s">
         <v>427</v>
       </c>
-      <c r="C74" t="s">
+      <c r="E74" t="s">
         <v>428</v>
       </c>
-      <c r="D74" t="s">
+      <c r="F74" t="s">
         <v>429</v>
       </c>
-      <c r="E74" t="s">
+      <c r="G74" t="s">
+        <v>143</v>
+      </c>
+      <c r="H74" t="s">
+        <v>119</v>
+      </c>
+      <c r="I74" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="F74" t="s">
+      <c r="L74" t="s">
         <v>431</v>
-      </c>
-      <c r="G74" t="s">
-        <v>144</v>
-      </c>
-      <c r="H74" t="s">
-        <v>120</v>
-      </c>
-      <c r="I74" t="s">
-        <v>16</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="L74" t="s">
-        <v>433</v>
       </c>
       <c r="M74" s="5">
         <v>44389</v>
@@ -5567,34 +5540,34 @@
         <v>73</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C75" t="s">
+        <v>433</v>
+      </c>
+      <c r="D75" t="s">
+        <v>433</v>
+      </c>
+      <c r="E75" t="s">
+        <v>434</v>
+      </c>
+      <c r="F75" t="s">
         <v>435</v>
       </c>
-      <c r="D75" t="s">
-        <v>435</v>
-      </c>
-      <c r="E75" t="s">
+      <c r="G75" t="s">
         <v>436</v>
       </c>
-      <c r="F75" t="s">
+      <c r="H75" t="s">
+        <v>119</v>
+      </c>
+      <c r="I75" t="s">
+        <v>16</v>
+      </c>
+      <c r="J75" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="G75" t="s">
+      <c r="L75" t="s">
         <v>438</v>
-      </c>
-      <c r="H75" t="s">
-        <v>120</v>
-      </c>
-      <c r="I75" t="s">
-        <v>16</v>
-      </c>
-      <c r="J75" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="L75" t="s">
-        <v>440</v>
       </c>
       <c r="M75" s="5">
         <v>43769</v>
@@ -5603,7 +5576,7 @@
         <v>150</v>
       </c>
       <c r="O75" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
@@ -5611,22 +5584,22 @@
         <v>74</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C76" t="s">
+        <v>441</v>
+      </c>
+      <c r="D76" t="s">
+        <v>442</v>
+      </c>
+      <c r="E76" t="s">
         <v>443</v>
       </c>
-      <c r="D76" t="s">
+      <c r="F76" t="s">
         <v>444</v>
       </c>
-      <c r="E76" t="s">
+      <c r="G76" t="s">
         <v>445</v>
-      </c>
-      <c r="F76" t="s">
-        <v>446</v>
-      </c>
-      <c r="G76" t="s">
-        <v>447</v>
       </c>
       <c r="H76" t="s">
         <v>15</v>
@@ -5635,10 +5608,10 @@
         <v>16</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M76" s="5">
         <v>43991</v>
@@ -5647,7 +5620,7 @@
         <v>40</v>
       </c>
       <c r="O76" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
@@ -5655,34 +5628,34 @@
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C77" t="s">
+        <v>447</v>
+      </c>
+      <c r="D77" t="s">
+        <v>448</v>
+      </c>
+      <c r="E77" t="s">
         <v>449</v>
       </c>
-      <c r="D77" t="s">
-        <v>450</v>
-      </c>
-      <c r="E77" t="s">
-        <v>451</v>
-      </c>
       <c r="F77" t="s">
+        <v>366</v>
+      </c>
+      <c r="G77" t="s">
         <v>367</v>
       </c>
-      <c r="G77" t="s">
-        <v>368</v>
-      </c>
       <c r="H77" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I77" t="s">
         <v>16</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="L77" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="M77" s="5">
         <v>43769</v>
@@ -5691,7 +5664,7 @@
         <v>100</v>
       </c>
       <c r="O77" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -5699,19 +5672,19 @@
         <v>76</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="C78" t="s">
+        <v>452</v>
+      </c>
+      <c r="D78" t="s">
         <v>453</v>
       </c>
-      <c r="C78" t="s">
+      <c r="E78" t="s">
         <v>454</v>
       </c>
-      <c r="D78" t="s">
+      <c r="F78" t="s">
         <v>455</v>
-      </c>
-      <c r="E78" t="s">
-        <v>456</v>
-      </c>
-      <c r="F78" t="s">
-        <v>457</v>
       </c>
       <c r="G78" t="s">
         <v>71</v>
@@ -5723,7 +5696,7 @@
         <v>16</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="M78" s="5">
         <v>44187</v>
@@ -5732,7 +5705,7 @@
         <v>35</v>
       </c>
       <c r="O78" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
@@ -5740,22 +5713,22 @@
         <v>77</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C79" t="s">
+        <v>458</v>
+      </c>
+      <c r="D79" t="s">
         <v>459</v>
       </c>
-      <c r="C79" t="s">
+      <c r="E79" t="s">
         <v>460</v>
       </c>
-      <c r="D79" t="s">
+      <c r="F79" t="s">
         <v>461</v>
       </c>
-      <c r="E79" t="s">
-        <v>462</v>
-      </c>
-      <c r="F79" t="s">
-        <v>463</v>
-      </c>
       <c r="G79" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H79" t="s">
         <v>27</v>
@@ -5764,7 +5737,7 @@
         <v>16</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="M79" s="5">
         <v>43647</v>
@@ -5773,7 +5746,7 @@
         <v>94</v>
       </c>
       <c r="O79" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -5781,19 +5754,19 @@
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C80" t="s">
+        <v>464</v>
+      </c>
+      <c r="D80" t="s">
+        <v>465</v>
+      </c>
+      <c r="E80" t="s">
         <v>466</v>
       </c>
-      <c r="D80" t="s">
+      <c r="F80" t="s">
         <v>467</v>
-      </c>
-      <c r="E80" t="s">
-        <v>468</v>
-      </c>
-      <c r="F80" t="s">
-        <v>469</v>
       </c>
       <c r="G80" t="s">
         <v>14</v>
@@ -5805,13 +5778,13 @@
         <v>16</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="M80" s="4">
         <v>43252</v>
       </c>
       <c r="O80" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
@@ -5819,34 +5792,34 @@
         <v>79</v>
       </c>
       <c r="B81" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C81" t="s">
+        <v>471</v>
+      </c>
+      <c r="D81" t="s">
         <v>472</v>
       </c>
-      <c r="C81" t="s">
+      <c r="E81" t="s">
         <v>473</v>
       </c>
-      <c r="D81" t="s">
+      <c r="F81" t="s">
         <v>474</v>
       </c>
-      <c r="E81" t="s">
+      <c r="G81" t="s">
         <v>475</v>
       </c>
-      <c r="F81" t="s">
+      <c r="H81" t="s">
         <v>476</v>
       </c>
-      <c r="G81" t="s">
+      <c r="I81" t="s">
+        <v>211</v>
+      </c>
+      <c r="J81" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="H81" t="s">
+      <c r="L81" t="s">
         <v>478</v>
-      </c>
-      <c r="I81" t="s">
-        <v>212</v>
-      </c>
-      <c r="J81" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="L81" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
@@ -5854,34 +5827,34 @@
         <v>80</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="C82" t="s">
+        <v>480</v>
+      </c>
+      <c r="D82" t="s">
         <v>481</v>
       </c>
-      <c r="C82" t="s">
+      <c r="E82" t="s">
         <v>482</v>
       </c>
-      <c r="D82" t="s">
+      <c r="F82" t="s">
         <v>483</v>
       </c>
-      <c r="E82" t="s">
+      <c r="G82" t="s">
+        <v>237</v>
+      </c>
+      <c r="H82" t="s">
+        <v>238</v>
+      </c>
+      <c r="I82" t="s">
+        <v>211</v>
+      </c>
+      <c r="J82" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="F82" t="s">
-        <v>485</v>
-      </c>
-      <c r="G82" t="s">
-        <v>238</v>
-      </c>
-      <c r="H82" t="s">
-        <v>239</v>
-      </c>
-      <c r="I82" t="s">
-        <v>212</v>
-      </c>
-      <c r="J82" s="3" t="s">
-        <v>486</v>
-      </c>
       <c r="L82" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M82" s="5">
         <v>43994</v>
@@ -5890,7 +5863,7 @@
         <v>135</v>
       </c>
       <c r="O82" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
@@ -5898,19 +5871,19 @@
         <v>81</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C83" t="s">
+        <v>487</v>
+      </c>
+      <c r="D83" t="s">
         <v>488</v>
       </c>
-      <c r="C83" t="s">
+      <c r="E83" t="s">
         <v>489</v>
       </c>
-      <c r="D83" t="s">
+      <c r="F83" t="s">
         <v>490</v>
-      </c>
-      <c r="E83" t="s">
-        <v>491</v>
-      </c>
-      <c r="F83" t="s">
-        <v>492</v>
       </c>
       <c r="G83" t="s">
         <v>26</v>
@@ -5922,10 +5895,10 @@
         <v>16</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L83" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="M83" s="5">
         <v>44012</v>
@@ -5934,7 +5907,7 @@
         <v>86</v>
       </c>
       <c r="O83" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
@@ -5942,34 +5915,34 @@
         <v>82</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="C84" t="s">
+        <v>495</v>
+      </c>
+      <c r="D84" t="s">
         <v>496</v>
       </c>
-      <c r="C84" t="s">
+      <c r="E84" t="s">
+        <v>165</v>
+      </c>
+      <c r="F84" t="s">
+        <v>166</v>
+      </c>
+      <c r="G84" t="s">
+        <v>84</v>
+      </c>
+      <c r="H84" t="s">
+        <v>85</v>
+      </c>
+      <c r="I84" t="s">
+        <v>16</v>
+      </c>
+      <c r="J84" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="D84" t="s">
-        <v>498</v>
-      </c>
-      <c r="E84" t="s">
-        <v>166</v>
-      </c>
-      <c r="F84" t="s">
-        <v>167</v>
-      </c>
-      <c r="G84" t="s">
-        <v>85</v>
-      </c>
-      <c r="H84" t="s">
-        <v>86</v>
-      </c>
-      <c r="I84" t="s">
-        <v>16</v>
-      </c>
-      <c r="J84" s="3" t="s">
-        <v>499</v>
-      </c>
       <c r="L84" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M84" s="5">
         <v>44310</v>
@@ -5978,7 +5951,7 @@
         <v>20</v>
       </c>
       <c r="O84" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
@@ -5986,19 +5959,19 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="C85" t="s">
+        <v>500</v>
+      </c>
+      <c r="D85" t="s">
         <v>501</v>
       </c>
-      <c r="C85" t="s">
-        <v>502</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>503</v>
       </c>
-      <c r="E85" t="s">
-        <v>505</v>
-      </c>
       <c r="F85" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G85" t="s">
         <v>63</v>
@@ -6010,10 +5983,10 @@
         <v>16</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="L85" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M85" s="5">
         <v>43658</v>
@@ -6022,7 +5995,7 @@
         <v>721</v>
       </c>
       <c r="O85" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
@@ -6030,19 +6003,19 @@
         <v>84</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="C86" t="s">
+        <v>505</v>
+      </c>
+      <c r="D86" t="s">
         <v>506</v>
       </c>
-      <c r="C86" t="s">
+      <c r="E86" t="s">
         <v>507</v>
       </c>
-      <c r="D86" t="s">
+      <c r="F86" t="s">
         <v>508</v>
-      </c>
-      <c r="E86" t="s">
-        <v>509</v>
-      </c>
-      <c r="F86" t="s">
-        <v>510</v>
       </c>
       <c r="G86" t="s">
         <v>14</v>
@@ -6054,13 +6027,13 @@
         <v>16</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="M86" s="5">
         <v>42856</v>
       </c>
       <c r="O86" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
@@ -6068,19 +6041,19 @@
         <v>85</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="C87" t="s">
+        <v>511</v>
+      </c>
+      <c r="D87" t="s">
         <v>512</v>
       </c>
-      <c r="C87" t="s">
-        <v>513</v>
-      </c>
-      <c r="D87" t="s">
-        <v>514</v>
-      </c>
       <c r="E87" t="s">
+        <v>152</v>
+      </c>
+      <c r="F87" t="s">
         <v>153</v>
-      </c>
-      <c r="F87" t="s">
-        <v>154</v>
       </c>
       <c r="G87" t="s">
         <v>71</v>
@@ -6092,10 +6065,10 @@
         <v>16</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="L87" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M87" s="5">
         <v>43991</v>
@@ -6104,7 +6077,7 @@
         <v>314</v>
       </c>
       <c r="O87" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
@@ -6112,34 +6085,34 @@
         <v>86</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="C88" t="s">
+        <v>515</v>
+      </c>
+      <c r="D88" t="s">
         <v>516</v>
       </c>
-      <c r="C88" t="s">
-        <v>517</v>
-      </c>
-      <c r="D88" t="s">
-        <v>518</v>
-      </c>
       <c r="E88" t="s">
+        <v>158</v>
+      </c>
+      <c r="F88" t="s">
         <v>159</v>
       </c>
-      <c r="F88" t="s">
-        <v>160</v>
-      </c>
       <c r="G88" t="s">
+        <v>94</v>
+      </c>
+      <c r="H88" t="s">
         <v>95</v>
       </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
+        <v>16</v>
+      </c>
+      <c r="J88" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I88" t="s">
-        <v>16</v>
-      </c>
-      <c r="J88" s="3" t="s">
+      <c r="L88" t="s">
         <v>97</v>
-      </c>
-      <c r="L88" t="s">
-        <v>98</v>
       </c>
       <c r="M88" s="5">
         <v>44306</v>
@@ -6148,7 +6121,7 @@
         <v>50</v>
       </c>
       <c r="O88" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
@@ -6156,40 +6129,40 @@
         <v>87</v>
       </c>
       <c r="B89" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="C89" t="s">
+        <v>519</v>
+      </c>
+      <c r="D89" t="s">
         <v>520</v>
       </c>
-      <c r="C89" t="s">
+      <c r="E89" t="s">
         <v>521</v>
       </c>
-      <c r="D89" t="s">
+      <c r="F89" t="s">
         <v>522</v>
       </c>
-      <c r="E89" t="s">
-        <v>523</v>
-      </c>
-      <c r="F89" t="s">
-        <v>524</v>
-      </c>
       <c r="G89" t="s">
+        <v>118</v>
+      </c>
+      <c r="H89" t="s">
         <v>119</v>
       </c>
-      <c r="H89" t="s">
-        <v>120</v>
-      </c>
       <c r="I89" t="s">
         <v>16</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="L89" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="M89" s="5">
         <v>43769</v>
       </c>
       <c r="O89" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="90" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -6197,19 +6170,19 @@
         <v>88</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C90" t="s">
+        <v>524</v>
+      </c>
+      <c r="D90" t="s">
+        <v>525</v>
+      </c>
+      <c r="E90" t="s">
         <v>526</v>
       </c>
-      <c r="D90" t="s">
+      <c r="F90" t="s">
         <v>527</v>
-      </c>
-      <c r="E90" t="s">
-        <v>528</v>
-      </c>
-      <c r="F90" t="s">
-        <v>529</v>
       </c>
       <c r="G90" t="s">
         <v>14</v>
@@ -6221,19 +6194,19 @@
         <v>16</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="L90" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M90" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="N90">
         <v>103</v>
       </c>
       <c r="O90" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -6241,34 +6214,34 @@
         <v>89</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C91" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D91" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E91" t="s">
+        <v>141</v>
+      </c>
+      <c r="F91" t="s">
         <v>142</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>143</v>
       </c>
-      <c r="G91" t="s">
-        <v>144</v>
-      </c>
       <c r="H91" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I91" t="s">
         <v>16</v>
       </c>
       <c r="J91" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="L91" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="L91" s="3" t="s">
-        <v>326</v>
       </c>
       <c r="M91" s="4">
         <v>43768</v>
@@ -6277,7 +6250,7 @@
         <v>519</v>
       </c>
       <c r="O91" s="3" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
@@ -6285,19 +6258,19 @@
         <v>90</v>
       </c>
       <c r="B92" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="C92" t="s">
+        <v>535</v>
+      </c>
+      <c r="D92" t="s">
         <v>536</v>
       </c>
-      <c r="C92" t="s">
+      <c r="E92" t="s">
         <v>537</v>
       </c>
-      <c r="D92" t="s">
-        <v>538</v>
-      </c>
-      <c r="E92" t="s">
-        <v>539</v>
-      </c>
       <c r="F92" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G92" t="s">
         <v>71</v>
@@ -6309,10 +6282,10 @@
         <v>16</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="L92" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M92" s="5">
         <v>44186</v>
@@ -6321,7 +6294,7 @@
         <v>116</v>
       </c>
       <c r="O92" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
@@ -6329,19 +6302,19 @@
         <v>91</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C93" t="s">
+        <v>535</v>
+      </c>
+      <c r="D93" t="s">
+        <v>540</v>
+      </c>
+      <c r="E93" t="s">
         <v>537</v>
       </c>
-      <c r="D93" t="s">
-        <v>542</v>
-      </c>
-      <c r="E93" t="s">
-        <v>539</v>
-      </c>
       <c r="F93" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G93" t="s">
         <v>71</v>
@@ -6353,10 +6326,10 @@
         <v>16</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="L93" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="M93" s="5">
         <v>44258</v>
@@ -6367,16 +6340,16 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
+        <v>535</v>
+      </c>
+      <c r="D94" t="s">
+        <v>541</v>
+      </c>
+      <c r="E94" t="s">
         <v>537</v>
       </c>
-      <c r="D94" t="s">
-        <v>543</v>
-      </c>
-      <c r="E94" t="s">
-        <v>539</v>
-      </c>
       <c r="F94" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G94" t="s">
         <v>71</v>
@@ -6393,34 +6366,34 @@
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="C95" t="s">
+        <v>542</v>
+      </c>
+      <c r="D95" t="s">
+        <v>543</v>
+      </c>
+      <c r="E95" t="s">
+        <v>544</v>
+      </c>
+      <c r="F95" t="s">
+        <v>545</v>
+      </c>
+      <c r="G95" t="s">
+        <v>546</v>
+      </c>
+      <c r="H95" t="s">
+        <v>210</v>
+      </c>
+      <c r="I95" t="s">
+        <v>211</v>
+      </c>
+      <c r="J95" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="L95" s="3" t="s">
         <v>613</v>
-      </c>
-      <c r="C95" t="s">
-        <v>544</v>
-      </c>
-      <c r="D95" t="s">
-        <v>545</v>
-      </c>
-      <c r="E95" t="s">
-        <v>546</v>
-      </c>
-      <c r="F95" t="s">
-        <v>547</v>
-      </c>
-      <c r="G95" t="s">
-        <v>548</v>
-      </c>
-      <c r="H95" t="s">
-        <v>211</v>
-      </c>
-      <c r="I95" t="s">
-        <v>212</v>
-      </c>
-      <c r="J95" s="3" t="s">
-        <v>561</v>
-      </c>
-      <c r="L95" s="3" t="s">
-        <v>616</v>
       </c>
       <c r="M95" s="4">
         <v>43809</v>
@@ -6429,7 +6402,7 @@
         <v>109</v>
       </c>
       <c r="O95" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>